<commit_message>
final code used for the testing of the dp4 dissertation
</commit_message>
<xml_diff>
--- a/feature_sorting/Actual_Battery_Centres.xlsx
+++ b/feature_sorting/Actual_Battery_Centres.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University_Year_4\DP4\DP4_FINAL\MODELLING\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\dp4\smartphone_inspection\feature_sorting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36257A60-9B9C-4E24-A44F-7C9ED2B22277}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8615A7FC-47F6-4E33-A758-6476BD4DF52A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CB5D5284-31D7-4C14-B533-4793F9897995}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="25">
   <si>
     <t>Phone_1</t>
   </si>
@@ -85,13 +85,37 @@
   </si>
   <si>
     <t>Battery Y</t>
+  </si>
+  <si>
+    <t>x (pixels)</t>
+  </si>
+  <si>
+    <t>y (pixels)</t>
+  </si>
+  <si>
+    <t>Exact Centre</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>Estimated Centre</t>
+  </si>
+  <si>
+    <t>Absolute Difference</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,8 +147,15 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -149,8 +180,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -290,23 +333,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -327,6 +389,56 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -335,8 +447,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF0000"/>
       <color rgb="FFFF9393"/>
-      <color rgb="FFFF0000"/>
     </mruColors>
   </colors>
   <extLst>
@@ -647,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6A01EB-4102-4448-BCA3-66FD8F53F055}">
-  <dimension ref="B1:M27"/>
+  <dimension ref="B1:V27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -663,455 +775,566 @@
     <col min="9" max="10" width="15.109375" customWidth="1"/>
     <col min="11" max="11" width="13.21875" customWidth="1"/>
     <col min="12" max="13" width="15.109375" customWidth="1"/>
+    <col min="16" max="16" width="17.5546875" customWidth="1"/>
+    <col min="20" max="20" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:13" ht="21" x14ac:dyDescent="0.4">
-      <c r="B2" s="3" t="s">
+    <row r="1" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:22" ht="21" x14ac:dyDescent="0.4">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="3" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="3" t="s">
+      <c r="F2" s="14"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="3" t="s">
+      <c r="I2" s="14"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="5"/>
-    </row>
-    <row r="3" spans="2:13" ht="18" x14ac:dyDescent="0.35">
-      <c r="B3" s="11" t="s">
+      <c r="L2" s="14"/>
+      <c r="M2" s="15"/>
+    </row>
+    <row r="3" spans="2:22" ht="18" x14ac:dyDescent="0.35">
+      <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="L3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="M3" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="12" t="s">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="3">
         <v>1915</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="4">
         <v>1771</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="3">
         <v>2038</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="4">
         <v>1638</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="3">
         <v>1825</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="4">
         <v>1457</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="3">
         <v>1959</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="4">
         <v>1895</v>
       </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="12" t="s">
+      <c r="P4" s="26"/>
+      <c r="Q4" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="R4" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="T4" s="26"/>
+      <c r="U4" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="V4" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="3">
         <v>1915</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="4">
         <v>1777</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="3">
         <v>2041</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="4">
         <v>1645</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="3">
         <v>1821</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="4">
         <v>1461</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="3">
         <v>1958</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="4">
         <v>1896</v>
       </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="12" t="s">
+      <c r="P5" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q5" s="18">
+        <v>1915</v>
+      </c>
+      <c r="R5" s="18">
+        <v>1771</v>
+      </c>
+      <c r="T5" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="U5" s="18">
+        <v>1915</v>
+      </c>
+      <c r="V5" s="18">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="3">
         <v>1915</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="4">
         <v>1771</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="3">
         <v>2039</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="4">
         <v>1640</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="3">
         <v>1822</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="4">
         <v>1457</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="3">
         <v>1954</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="4">
         <v>1906</v>
       </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="12" t="s">
+      <c r="P6" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q6" s="21">
+        <v>1924</v>
+      </c>
+      <c r="R6" s="21">
+        <v>1780</v>
+      </c>
+      <c r="T6" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="U6" s="21">
+        <v>1926</v>
+      </c>
+      <c r="V6" s="21">
+        <v>1772</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="3">
         <v>1915</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="4">
         <v>1769</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="3">
         <v>2041</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="4">
         <v>1639</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="3">
         <v>1821</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="4">
         <v>1454</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="3">
         <v>1953</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="4">
         <v>1899</v>
       </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="12" t="s">
+      <c r="P7" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q7" s="25">
+        <f>Q6-Q5</f>
         <v>9</v>
       </c>
-      <c r="C8" s="6">
+      <c r="R7" s="25">
+        <f>R6-R5</f>
+        <v>9</v>
+      </c>
+      <c r="T7" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="U7" s="21">
+        <f>U6-U5</f>
+        <v>11</v>
+      </c>
+      <c r="V7" s="21">
+        <f>V6-V5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3">
         <v>1919</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="4">
         <v>1773</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="3">
         <v>2038</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="4">
         <v>1641</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="3">
         <v>1822</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="4">
         <v>1459</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="K8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="3">
         <v>1961</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="4">
         <v>1901</v>
       </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="12" t="s">
+      <c r="P8" s="22"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
+      <c r="T8" s="22"/>
+      <c r="U8" s="23"/>
+      <c r="V8" s="23"/>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="3">
         <v>1911</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="4">
         <v>1769</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="3">
         <v>2037</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="4">
         <v>1639</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="3">
         <v>1822</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="4">
         <v>1458</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L9" s="6">
+      <c r="L9" s="3">
         <v>1958</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="4">
         <v>1896</v>
       </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="12" t="s">
+      <c r="P9" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q9" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="R9" s="28"/>
+      <c r="T9" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="U9" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="V9" s="29"/>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="3">
         <v>1915</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="4">
         <v>1765</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="3">
         <v>2036</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="4">
         <v>1639</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="3">
         <v>1822</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="4">
         <v>1456</v>
       </c>
-      <c r="K10" s="12" t="s">
+      <c r="K10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L10" s="3">
         <v>1956</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="4">
         <v>1901</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="12" t="s">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="3">
         <v>1915</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="4">
         <v>1771</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="3">
         <v>2037</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="4">
         <v>1643</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="3">
         <v>1821</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="4">
         <v>1458</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L11" s="3">
         <v>1962</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="4">
         <v>1895</v>
       </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="12" t="s">
+      <c r="P11" s="22"/>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="30"/>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="3">
         <v>1913</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="4">
         <v>1768</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="3">
         <v>2038</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="4">
         <v>1643</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="H12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="3">
         <v>1821</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="4">
         <v>1459</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="K12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="L12" s="6">
+      <c r="L12" s="3">
         <v>1961</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="4">
         <v>1890</v>
       </c>
-    </row>
-    <row r="13" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="13" t="s">
+      <c r="P12" s="22"/>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="31"/>
+    </row>
+    <row r="13" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="5">
         <v>1913</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="6">
         <v>1765</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="5">
         <v>2036</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="7">
         <v>1642</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="5">
         <v>1820</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="6">
         <v>1450</v>
       </c>
-      <c r="K13" s="13" t="s">
+      <c r="K13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L13" s="5">
         <v>1965</v>
       </c>
-      <c r="M13" s="9">
+      <c r="M13" s="6">
         <v>1893</v>
       </c>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P13" s="22"/>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="31"/>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="P14" s="22"/>
+      <c r="Q14" s="31"/>
+      <c r="R14" s="31"/>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P15" s="22"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="22"/>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1124,6 +1347,9 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
+      <c r="P16" s="22"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="32"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
@@ -1169,8 +1395,8 @@
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -1183,8 +1409,8 @@
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1274,11 +1500,14 @@
       <c r="M27" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="Q16:R16"/>
+    <mergeCell ref="U9:V9"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:M2"/>
+    <mergeCell ref="Q9:R9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>